<commit_message>
assets: :bento: updated import excel template on commodity location
</commit_message>
<xml_diff>
--- a/public/import-ruangan-template.xlsx
+++ b/public/import-ruangan-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11A5614-B2AD-4500-A7AE-9AEDE9E44720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAC05E7-5497-4BB0-AF55-18C920AB0C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -351,13 +354,13 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>